<commit_message>
Complete the actual list of the pn description
</commit_message>
<xml_diff>
--- a/Prometheus/Prometheus/Scripts/project_pn_desc_list.xlsx
+++ b/Prometheus/Prometheus/Scripts/project_pn_desc_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>QSFP28 SR4</t>
   </si>
@@ -190,6 +190,102 @@
   </si>
   <si>
     <t>If you can not find the data which you want,please contact Brad.Qiu</t>
+  </si>
+  <si>
+    <t>FTLC9141</t>
+  </si>
+  <si>
+    <t> FCBN425QE; FCBN425QB; FCBR425QB</t>
+  </si>
+  <si>
+    <t> FCBN425QP</t>
+  </si>
+  <si>
+    <t>FBOTD25SL</t>
+  </si>
+  <si>
+    <t>FBOTD25FL3</t>
+  </si>
+  <si>
+    <t>FBOTD25FL2</t>
+  </si>
+  <si>
+    <t>FTLC8221</t>
+  </si>
+  <si>
+    <t>FCBG125SD1;FCCG125SD1;FCBN125SD1;FCCN125SD1</t>
+  </si>
+  <si>
+    <t>FCBG110SD2;FCBN125SD1</t>
+  </si>
+  <si>
+    <t>FCBG110SD1</t>
+  </si>
+  <si>
+    <t>FCCG410QD3;FCBG410QD3;FCBN410QD3;FCCN410QD3;FCCG414QD3;FCBG414QD3;FCBN414QD3;FCCN414QD3</t>
+  </si>
+  <si>
+    <t>FTL410QD1;FTL410QE1;FTL410QX1</t>
+  </si>
+  <si>
+    <t>FTL410QD2;FTL410QE2;FTL410QX2</t>
+  </si>
+  <si>
+    <t>FTL410QD3;FTL410QE3;FTL410QX3</t>
+  </si>
+  <si>
+    <t>FTL410QD4;FTL410QE4;FTL410QX4</t>
+  </si>
+  <si>
+    <t>FTLD10CE3;FTLD10CD3</t>
+  </si>
+  <si>
+    <t>FCBND10CD3</t>
+  </si>
+  <si>
+    <t>FCBND12CD1</t>
+  </si>
+  <si>
+    <t>FCBND12CD3</t>
+  </si>
+  <si>
+    <t>FTLD12CL3</t>
+  </si>
+  <si>
+    <t>FTLD10CX1</t>
+  </si>
+  <si>
+    <t>FCBND10CD1;FCBRD10CD1</t>
+  </si>
+  <si>
+    <t>FCBN410QB1</t>
+  </si>
+  <si>
+    <t>FCBN410QE2</t>
+  </si>
+  <si>
+    <t>QSFP28 SR4 LP</t>
+  </si>
+  <si>
+    <t>QSFP28 SR4 Gen2</t>
+  </si>
+  <si>
+    <t>FTLC9553</t>
+  </si>
+  <si>
+    <t>QSFP28 SR4 Error Free</t>
+  </si>
+  <si>
+    <t>FTLC9554</t>
+  </si>
+  <si>
+    <t>FTLC9552</t>
+  </si>
+  <si>
+    <t>FTLC9551</t>
+  </si>
+  <si>
+    <t>FBOPD10SL1;FBOTD10FL1;FBOTD10SE1;FBOTD10SH1;FBOTD10SM1;FBOTD10SL1</t>
   </si>
 </sst>
 </file>
@@ -541,16 +637,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="100.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -570,226 +668,334 @@
       <c r="B2" t="s">
         <v>29</v>
       </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>